<commit_message>
Save changes to __state_count_stats_by_year.xlsx before switching branches
</commit_message>
<xml_diff>
--- a/_extra/__state_count_stats_by_year.xlsx
+++ b/_extra/__state_count_stats_by_year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mr_Green\OneDrive\Desktop\0_Sum_25\INFO_526\project-final\_extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D9B1DE75-79D8-4FCD-933E-5A9EA01EA6D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{5D50E633-9FC2-408F-A92F-330CA2D14A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4095" yWindow="1845" windowWidth="28230" windowHeight="13290" xr2:uid="{1857DBB9-35C0-494F-B92A-C301AB5A114D}"/>
+    <workbookView xWindow="-3270" yWindow="9315" windowWidth="28230" windowHeight="13290" xr2:uid="{1857DBB9-35C0-494F-B92A-C301AB5A114D}"/>
   </bookViews>
   <sheets>
     <sheet name="state_count_stats_by_year" sheetId="1" r:id="rId1"/>
@@ -1108,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE87F01-73D1-494F-A995-9C3B0933C4A5}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>